<commit_message>
updated tasks for A1-A6
</commit_message>
<xml_diff>
--- a/JianHongHong/evidence.xlsx
+++ b/JianHongHong/evidence.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" state="visible" r:id="rId2"/>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Jax | StakeWithUs#8830, YH | StakeWithUs#6077</t>
   </si>
   <si>
-    <t xml:space="preserve">set none if no community</t>
+    <t xml:space="preserve">none</t>
   </si>
   <si>
     <t xml:space="preserve">TxHash</t>
@@ -100,76 +100,58 @@
     <t xml:space="preserve">ClassID</t>
   </si>
   <si>
-    <t xml:space="preserve">D9A2E572E01A605C1B6FEADD1D40C2FE9836ACF0769CEB399C86518E07F86CBB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">swugon</t>
+    <t xml:space="preserve">681B53B42A84FD4EA0EE4CD86665BC14E740A115AD1216D6FB9A5AFF389CB7B5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swuCollections</t>
   </si>
   <si>
     <t xml:space="preserve">NFTID</t>
   </si>
   <si>
-    <t xml:space="preserve">D186E9F7B6C96764FA68F1C82EF8263BB88CF24612EA8025BA924C37B9CED4AA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">swunft</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DBF674E3288D8D95746259DF025861C080CB037E0A193F81962D0AC668F06E18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">swunft1</t>
+    <t xml:space="preserve">51B2C9887CA24C5598B41DFF095D08F71882A8E59FDCB274C7BCD420B6CF7832</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swuNFT1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">079DED34620988E9FB8DE8F2BC13E34BA53BE8A5C321072D67C28D1CFF18FD56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">swuNFT2</t>
   </si>
   <si>
     <t xml:space="preserve">ChainID</t>
   </si>
   <si>
-    <t xml:space="preserve">69C68011B14BD385DF409539F4A0B4D4678B706CCB46F11020849BA38787274C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wasm.stars1ve46fjrhcrum94c7d8yc2wsdz8cpuw73503e8qn9r44spr6dw0lsvmvtqh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Elgafar-1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E19C6B2BB696F03AE8AD42325185343CF34331452C7219B4F098BD4ACF44D75B</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">ibc/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">45C0E30158DCE496D0A65D0C5D581C4EC3FBD3255592CCDACA1B327545CFF0FD</t>
-    </r>
+    <t xml:space="preserve">8E1C0486695A3CA6BD9EBDF2D2AC67FFCA13ABFF12201AE65AE97E94C8A7AFE7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">stars1cpd8fvkaak2gzjz2w5wnvmvspxkw76j4fut78qlcas3vdpcc4slqrs6f7q</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elgafar-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1D3701F97594EF333B989AC85B46E52F88B3ED0E96DA28BFAED47D488AFA475C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ibc/9D304CD58D226681323425C4FCCD224C2F5B4E05EDF47C11D3CC118E841A5A24</t>
   </si>
   <si>
     <t xml:space="preserve">uptick_7000-2</t>
   </si>
   <si>
-    <t xml:space="preserve">tx hash on dest chain</t>
+    <t xml:space="preserve">AC7AB3955B31D47182982DF3DAA1CBC67055C1F2F3CB10E6DE2242BD4EFD23E8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5E8B98769B4F9BCAC9F440C8E1DF696F1E25A0ADE48A3E9FA1765776DB7FDA03</t>
   </si>
   <si>
     <t xml:space="preserve">ibc class on chain</t>
   </si>
   <si>
     <t xml:space="preserve">nft id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dest chain id</t>
   </si>
   <si>
     <t xml:space="preserve">tx hash on that chain</t>
@@ -194,7 +176,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -229,12 +211,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
   </fonts>
   <fills count="4">
@@ -306,7 +282,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -335,12 +311,8 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -423,7 +395,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="M6" activeCellId="0" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -528,10 +500,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -572,10 +544,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -616,10 +588,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -660,10 +632,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1009,7 +981,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1365,61 +1337,61 @@
       <c r="A3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
-      <c r="D4" s="8"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
-      <c r="D5" s="8"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
-      <c r="D6" s="8"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
-      <c r="D7" s="8"/>
+      <c r="D7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6"/>
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="8"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
-      <c r="D9" s="8"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6"/>
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
-      <c r="D10" s="8"/>
+      <c r="D10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
-      <c r="D11" s="8"/>
+      <c r="D11" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1440,7 +1412,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1497,16 +1469,16 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="82.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="72.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="99.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1556,14 +1528,15 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.43"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="84.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="80.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="37.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1584,14 +1557,14 @@
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>33</v>
+      <c r="B2" s="7" t="s">
+        <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>35</v>
+        <v>22</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1612,14 +1585,14 @@
   </sheetPr>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.01"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="95.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="96.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.43"/>
   </cols>
@@ -1640,16 +1613,16 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="5" t="s">
         <v>33</v>
       </c>
+      <c r="B2" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="C2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>35</v>
+        <v>24</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1690,10 +1663,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1734,10 +1707,10 @@
     </row>
     <row r="2" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>